<commit_message>
Update: airloads now correct
</commit_message>
<xml_diff>
--- a/initialization/TecnamP92_input.xlsx
+++ b/initialization/TecnamP92_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claum\OneDrive\Desktop\TesiMagistrale\tesi-magistrale-claudio-mirabella\initialization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EA95E9-DB0C-4C65-9591-33A960E7D2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE38B6F5-FEED-4698-8225-CF384138E962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{CE78F296-029D-4319-9163-0EA223876FFB}"/>
   </bookViews>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Regulation</t>
-  </si>
-  <si>
-    <t>CSVLA</t>
   </si>
   <si>
     <t>Date</t>
@@ -1190,6 +1187,9 @@
   </si>
   <si>
     <t>Wing semispan percentage</t>
+  </si>
+  <si>
+    <t>csvla</t>
   </si>
 </sst>
 </file>
@@ -1840,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B8085C-DBEF-4A79-B728-1C6218494374}">
   <dimension ref="A1:D220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,7 +1869,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -1907,7 +1907,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>288</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>8</v>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9">
         <v>43427</v>
@@ -1928,10 +1928,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>8</v>
@@ -1952,10 +1952,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>8</v>
@@ -1964,669 +1964,669 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="13">
         <v>450</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="14">
         <v>281</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="14">
         <v>169</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="14">
         <v>50.5</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="14">
         <v>180</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="17">
         <v>1.85</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="41">
         <v>0</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B17" s="41">
         <v>2000</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="43">
         <v>4000</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="42"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="45">
         <v>0.23</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20" s="45">
         <v>0.26</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="46"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="47">
         <v>0.25</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="91"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>27</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>28</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="19">
         <v>13.4</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="19">
         <v>9.6199999999999992</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="19">
         <v>1.5</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="19">
         <f>B10/B23</f>
         <v>33.582089552238806</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="19">
         <v>0.25</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="19">
+        <v>0.33</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="B28" s="19">
-        <v>0.125</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="19">
-        <v>0.4375</v>
+        <v>0.33</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="19">
-        <v>0.4375</v>
+        <v>0.33</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32" s="21"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" s="21"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="22">
         <v>0</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="21"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="22">
         <v>0</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="21"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="22">
         <v>0</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="21"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="22">
         <v>1.5</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="22">
         <v>1.5</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="22">
         <v>1.5</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" s="21"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" s="22">
         <v>-1.5</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="21"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="22">
         <v>-1.5</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="21"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="22">
         <v>-1.5</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="22">
         <v>-1.5</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="21"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" s="22">
         <v>0.25</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="22">
         <v>1.4</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47" s="22">
         <v>1.4</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="22">
         <v>1.4</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D48" s="21"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" s="22">
         <v>1.4</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D49" s="21"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="22">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D50" s="21"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B51" s="22">
         <v>0.4</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D51" s="21"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52" s="22">
         <v>0.12</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D52" s="21"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" s="22">
         <v>0</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D53" s="21"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="22">
         <v>0</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D54" s="21"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="22">
         <v>1.6379999999999999</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D55" s="21"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" s="22">
         <v>0</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D56" s="21"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" s="23">
         <v>0.16500000000000001</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" s="21"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B58" s="63">
         <v>6.3</v>
       </c>
       <c r="C58" s="63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B59" s="63">
         <v>1.1000000000000001</v>
       </c>
       <c r="C59" s="63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D59" s="64"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B60" s="63">
         <v>2.5</v>
       </c>
       <c r="C60" s="63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D60" s="64"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B61" s="63">
         <v>1.4</v>
       </c>
       <c r="C61" s="63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D61" s="64"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B62" s="84" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C62" s="63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D62" s="64"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B63" s="63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C63" s="63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D63" s="64"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="63" t="s">
+        <v>198</v>
+      </c>
+      <c r="B64" s="63" t="s">
         <v>199</v>
-      </c>
-      <c r="B64" s="63" t="s">
-        <v>200</v>
       </c>
       <c r="C64" s="63" t="s">
         <v>8</v>
@@ -2635,10 +2635,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="65" t="s">
+        <v>200</v>
+      </c>
+      <c r="B65" s="65" t="s">
         <v>201</v>
-      </c>
-      <c r="B65" s="65" t="s">
-        <v>202</v>
       </c>
       <c r="C65" s="65" t="s">
         <v>8</v>
@@ -2647,132 +2647,132 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B66" s="66">
         <v>1.97</v>
       </c>
       <c r="C66" s="66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B67" s="66">
         <v>2.9</v>
       </c>
       <c r="C67" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D67" s="67"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="66" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B68" s="66">
         <v>0.68</v>
       </c>
       <c r="C68" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D68" s="67"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B69" s="66">
         <v>0.68</v>
       </c>
       <c r="C69" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D69" s="67"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B70" s="66">
         <v>3.78</v>
       </c>
       <c r="C70" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D70" s="67"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B71" s="66">
         <v>0</v>
       </c>
       <c r="C71" s="66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D71" s="67"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B72" s="66">
         <v>0.2</v>
       </c>
       <c r="C72" s="66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D72" s="67"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B73" s="66">
         <v>0.12</v>
       </c>
       <c r="C73" s="66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D73" s="67"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74" s="66">
         <v>0</v>
       </c>
       <c r="C74" s="66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D74" s="67"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B75" s="66">
         <v>0.25</v>
       </c>
       <c r="C75" s="66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D75" s="67"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="66" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B76" s="66" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C76" s="66" t="s">
         <v>8</v>
@@ -2781,237 +2781,237 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B77" s="66">
         <v>6</v>
       </c>
       <c r="C77" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D77" s="67"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B78" s="66">
         <v>0</v>
       </c>
       <c r="C78" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D78" s="67"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B79" s="66">
         <v>0.15</v>
       </c>
       <c r="C79" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D79" s="67"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B80" s="66">
         <v>1.49</v>
       </c>
       <c r="C80" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D80" s="67"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B81" s="66">
         <v>0.3</v>
       </c>
       <c r="C81" s="66" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D81" s="67"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="66" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B82" s="66">
         <v>0</v>
       </c>
       <c r="C82" s="66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D82" s="67"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="66" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B83" s="66">
         <v>0</v>
       </c>
       <c r="C83" s="66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D83" s="67"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="66" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B84" s="66">
         <v>1</v>
       </c>
       <c r="C84" s="66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D84" s="67"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="68" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B85" s="68">
         <v>0</v>
       </c>
       <c r="C85" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D85" s="67"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B86" s="52">
         <v>0.72</v>
       </c>
       <c r="C86" s="70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D86" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B87" s="52">
         <v>1.23</v>
       </c>
       <c r="C87" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D87" s="53"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B88" s="52">
         <v>1</v>
       </c>
       <c r="C88" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D88" s="53"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="52" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B89" s="52">
         <v>0.47599999999999998</v>
       </c>
       <c r="C89" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D89" s="53"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B90" s="52">
         <v>0.68</v>
       </c>
       <c r="C90" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D90" s="53"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="52" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B91" s="52">
         <v>3.2</v>
       </c>
       <c r="C91" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D91" s="53"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="52" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B92" s="52">
         <v>15</v>
       </c>
       <c r="C92" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D92" s="53"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B93" s="52">
         <v>0</v>
       </c>
       <c r="C93" s="52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D93" s="53"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="52" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B94" s="52">
         <v>0</v>
       </c>
       <c r="C94" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D94" s="53"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B95" s="52">
         <v>0.2335363</v>
       </c>
       <c r="C95" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D95" s="53"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="52" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B96" s="52">
         <v>2</v>
@@ -3023,330 +3023,330 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="52" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B97" s="52">
         <v>0</v>
       </c>
       <c r="C97" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D97" s="53"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B98" s="52">
         <v>0</v>
       </c>
       <c r="C98" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D98" s="53"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="52" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B99" s="52">
         <v>0</v>
       </c>
       <c r="C99" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D99" s="53"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B100" s="52">
         <v>0.95</v>
       </c>
       <c r="C100" s="52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D100" s="53"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B101" s="52">
         <v>0</v>
       </c>
       <c r="C101" s="52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D101" s="53"/>
     </row>
     <row r="102" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="52" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B102" s="52">
         <v>1</v>
       </c>
       <c r="C102" s="52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D102" s="53"/>
     </row>
     <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="52" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B103" s="52">
         <v>1</v>
       </c>
       <c r="C103" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D103" s="53"/>
     </row>
     <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="52" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B104" s="52">
         <v>15</v>
       </c>
       <c r="C104" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D104" s="53"/>
     </row>
     <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B105" s="52">
         <v>20</v>
       </c>
       <c r="C105" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D105" s="53"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B106" s="52">
         <v>0</v>
       </c>
       <c r="C106" s="52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D106" s="53"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="54" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B107" s="54">
         <v>0</v>
       </c>
       <c r="C107" s="55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D107" s="53"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B108" s="48">
         <v>0.71399999999999997</v>
       </c>
       <c r="C108" s="48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D108" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B109" s="48">
         <v>1.97</v>
       </c>
       <c r="C109" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D109" s="49"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B110" s="48">
         <v>0.50309999999999999</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D110" s="49"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B111" s="48">
         <v>0.91269999999999996</v>
       </c>
       <c r="C111" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D111" s="49"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B112" s="48">
         <f>B116</f>
         <v>0.39004</v>
       </c>
       <c r="C112" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D112" s="49"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B113" s="48">
         <f>B116</f>
         <v>0.39004</v>
       </c>
       <c r="C113" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D113" s="49"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B114" s="48">
         <v>0.27860000000000001</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D114" s="49"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B115" s="48">
         <v>0.27860000000000001</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D115" s="49"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B116" s="48">
         <f>B48*B114</f>
         <v>0.39004</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D116" s="49"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B117" s="48">
         <f>B48*B115</f>
         <v>0.39004</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D117" s="49"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B118" s="50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C118" s="51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D118" s="49"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B119" s="52">
         <v>1.97</v>
       </c>
       <c r="C119" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D119" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B120" s="52">
         <v>2.9</v>
       </c>
       <c r="C120" s="52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D120" s="53"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B121" s="52">
         <v>0</v>
       </c>
       <c r="C121" s="52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D121" s="53"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B122" s="52">
         <v>1</v>
       </c>
       <c r="C122" s="52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D122" s="53"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B123" s="52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C123" s="52" t="s">
         <v>8</v>
@@ -3355,272 +3355,272 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B124" s="52">
         <f>0.68/B68</f>
         <v>1</v>
       </c>
       <c r="C124" s="52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D124" s="53"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B125" s="52">
         <f>0.68/B69</f>
         <v>1</v>
       </c>
       <c r="C125" s="52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D125" s="53"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B126" s="52">
         <f>0.75*B119</f>
         <v>1.4775</v>
       </c>
       <c r="C126" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D126" s="53"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B127" s="54">
         <v>3.78</v>
       </c>
       <c r="C127" s="55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D127" s="53"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B128" s="56">
         <v>0.35</v>
       </c>
       <c r="C128" s="56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D128" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B129" s="56">
         <v>1</v>
       </c>
       <c r="C129" s="56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D129" s="57"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="56" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B130" s="56">
         <v>0.1</v>
       </c>
       <c r="C130" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D130" s="57"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B131" s="56">
         <v>0.9</v>
       </c>
       <c r="C131" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D131" s="57"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B132" s="56">
         <v>0.63</v>
       </c>
       <c r="C132" s="56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D132" s="57"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B133" s="56">
         <v>0.48</v>
       </c>
       <c r="C133" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D133" s="57"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B134" s="56">
         <v>0.8</v>
       </c>
       <c r="C134" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D134" s="57"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B135" s="56">
         <f>B132/B48</f>
         <v>0.45</v>
       </c>
       <c r="C135" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D135" s="57"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B136" s="56">
         <f>B132/B48</f>
         <v>0.45</v>
       </c>
       <c r="C136" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D136" s="57"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B137" s="58">
         <v>3.2</v>
       </c>
       <c r="C137" s="59" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D137" s="57"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B138" s="60">
         <v>0.21072869999999999</v>
       </c>
       <c r="C138" s="60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B139" s="60">
         <v>1.365</v>
       </c>
       <c r="C139" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D139" s="61"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="60" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B140" s="60">
         <f>(2*0.26/B24)</f>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="C140" s="92" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D140" s="61"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="60" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B141" s="60">
         <v>0.50119999999999998</v>
       </c>
       <c r="C141" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D141" s="61"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B142" s="60">
         <v>0.27860000000000001</v>
       </c>
       <c r="C142" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D142" s="61"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B143" s="60">
         <v>0.27860000000000001</v>
       </c>
       <c r="C143" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D143" s="61"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B144" s="60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C144" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D144" s="61"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="B145" s="62" t="s">
         <v>190</v>
-      </c>
-      <c r="B145" s="62" t="s">
-        <v>191</v>
       </c>
       <c r="C145" s="62" t="s">
         <v>8</v>
@@ -3629,815 +3629,815 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="71" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B146" s="71">
         <v>0.12</v>
       </c>
       <c r="C146" s="71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="72" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B147" s="72">
         <v>0.12</v>
       </c>
       <c r="C147" s="73" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D147" s="74"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B148" s="36">
         <v>1.55</v>
       </c>
       <c r="C148" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D148" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B149" s="36">
         <v>1.9</v>
       </c>
       <c r="C149" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D149" s="37"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B150" s="36">
         <v>2.2000000000000002</v>
       </c>
       <c r="C150" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D150" s="37"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B151" s="36">
         <v>-1</v>
       </c>
       <c r="C151" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D151" s="37"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B152" s="36">
         <v>4.3600000000000003</v>
       </c>
       <c r="C152" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D152" s="37"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B153" s="36">
         <v>0</v>
       </c>
       <c r="C153" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D153" s="37"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B154" s="36">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="C154" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D154" s="37"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B155" s="36">
         <v>0.01</v>
       </c>
       <c r="C155" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D155" s="37"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B156" s="36">
         <v>0.8</v>
       </c>
       <c r="C156" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D156" s="37"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B157" s="36">
         <v>0.6</v>
       </c>
       <c r="C157" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D157" s="37"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B158" s="36">
         <v>1.3878999999999999</v>
       </c>
       <c r="C158" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D158" s="37"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B159" s="36">
         <v>-1.6541E-2</v>
       </c>
       <c r="C159" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D159" s="37"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B160" s="36">
         <v>0</v>
       </c>
       <c r="C160" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D160" s="37"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B161" s="36">
         <v>-0.16969999999999999</v>
       </c>
       <c r="C161" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D161" s="37"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B162" s="36">
         <v>-6.0999999999999999E-2</v>
       </c>
       <c r="C162" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D162" s="37"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B163" s="36">
         <v>-0.41</v>
       </c>
       <c r="C163" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D163" s="37"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B164" s="36">
         <v>-0.46100000000000002</v>
       </c>
       <c r="C164" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D164" s="37"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B165" s="36">
         <v>-0.26900000000000002</v>
       </c>
       <c r="C165" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D165" s="37"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B166" s="36">
         <v>-0.45</v>
       </c>
       <c r="C166" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D166" s="37"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B167" s="36">
         <v>-2.3999999999999998E-3</v>
       </c>
       <c r="C167" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D167" s="37"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B168" s="36">
         <v>30</v>
       </c>
       <c r="C168" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D168" s="37"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B169" s="36">
         <v>25</v>
       </c>
       <c r="C169" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D169" s="37"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B170" s="36">
         <v>25</v>
       </c>
       <c r="C170" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D170" s="37"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B171" s="36">
         <v>25</v>
       </c>
       <c r="C171" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D171" s="37"/>
     </row>
     <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B172" s="38" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C172" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D172" s="37"/>
     </row>
     <row r="173" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B173" s="38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C173" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D173" s="37"/>
     </row>
     <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B174" s="82" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C174" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D174" s="37"/>
     </row>
     <row r="175" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B175" s="83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C175" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D175" s="36"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="75" t="s">
+        <v>250</v>
+      </c>
+      <c r="B176" s="75" t="s">
         <v>251</v>
       </c>
-      <c r="B176" s="75" t="s">
+      <c r="C176" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="D176" s="32" t="s">
         <v>252</v>
-      </c>
-      <c r="C176" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="D176" s="32" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="75" t="s">
+        <v>253</v>
+      </c>
+      <c r="B177" s="75" t="s">
         <v>254</v>
       </c>
-      <c r="B177" s="75" t="s">
-        <v>255</v>
-      </c>
       <c r="C177" s="75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D177" s="76"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="75" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B178" s="77">
         <v>3.6156899999999999E-5</v>
       </c>
       <c r="C178" s="75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D178" s="76"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="75" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B179" s="75">
         <v>6.4400000000000004E-4</v>
       </c>
       <c r="C179" s="75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D179" s="76"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="75" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B180" s="75">
         <v>2.5399999999999999E-2</v>
       </c>
       <c r="C180" s="75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D180" s="76"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="75" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B181" s="75">
         <v>2.3300000000000001E-2</v>
       </c>
       <c r="C181" s="75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D181" s="76"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="78" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B182" s="78">
         <v>0.3</v>
       </c>
       <c r="C182" s="79" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D182" s="76"/>
     </row>
     <row r="183" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B183" s="65">
         <v>47.222200000000001</v>
       </c>
       <c r="C183" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="D183" s="80" t="s">
         <v>262</v>
-      </c>
-      <c r="D183" s="80" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="66" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B184" s="66">
         <v>3.8</v>
       </c>
       <c r="C184" s="66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D184" s="32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="66" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B185" s="66">
         <v>-1.5</v>
       </c>
       <c r="C185" s="66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D185" s="67"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="66" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B186" s="66">
         <v>15.24</v>
       </c>
       <c r="C186" s="66" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D186" s="67"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="68" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B187" s="68">
         <v>7.62</v>
       </c>
       <c r="C187" s="68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D187" s="81"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B188" s="26" t="s">
         <v>74</v>
-      </c>
-      <c r="B188" s="26" t="s">
-        <v>75</v>
       </c>
       <c r="C188" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B189" s="26">
         <v>4</v>
       </c>
       <c r="C189" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D189" s="27"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B190" s="28">
         <v>74.569999999999993</v>
       </c>
       <c r="C190" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D190" s="27"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B191" s="26">
         <v>5800</v>
       </c>
       <c r="C191" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D191" s="27"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B192" s="28">
         <v>2.4285999999999999</v>
       </c>
       <c r="C192" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D192" s="27"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B193" s="28">
         <f>B190*0.9</f>
         <v>67.113</v>
       </c>
       <c r="C193" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D193" s="27"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B194" s="26">
         <v>5500</v>
       </c>
       <c r="C194" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D194" s="29"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B195" s="26">
         <v>1.33</v>
       </c>
       <c r="C195" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D195" s="29"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B196" s="28">
         <v>15</v>
       </c>
       <c r="C196" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D196" s="29"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B197" s="28">
         <v>75</v>
       </c>
       <c r="C197" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D197" s="29"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B198" s="26">
         <v>1</v>
       </c>
       <c r="C198" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D198" s="29"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B199" s="26">
         <v>2.5</v>
       </c>
       <c r="C199" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D199" s="29"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B200" s="26">
         <v>2.5</v>
       </c>
       <c r="C200" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D200" s="29"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B201" s="26">
         <v>0</v>
       </c>
       <c r="C201" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D201" s="29"/>
     </row>
     <row r="202" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B202" s="26">
         <v>35</v>
       </c>
       <c r="C202" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D202" s="29"/>
     </row>
     <row r="203" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B203" s="26">
         <v>70</v>
       </c>
       <c r="C203" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D203" s="29"/>
     </row>
     <row r="204" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B204" s="26">
         <v>2.5</v>
       </c>
       <c r="C204" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D204" s="29"/>
     </row>
     <row r="205" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B205" s="85">
         <v>60</v>
       </c>
       <c r="C205" s="85" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D205" s="29"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="85" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B206" s="85">
         <v>0</v>
       </c>
       <c r="C206" s="85" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D206" s="29"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="85" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B207" s="85">
         <v>0</v>
       </c>
       <c r="C207" s="85" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D207" s="29"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="85" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B208" s="85">
         <v>0</v>
       </c>
       <c r="C208" s="85" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D208" s="29"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="85" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B209" s="85">
         <v>1.2</v>
       </c>
       <c r="C209" s="85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D209" s="29"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="85" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B210" s="85">
         <v>0.8</v>
       </c>
       <c r="C210" s="85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D210" s="29"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="85" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B211" s="85">
         <v>1.6</v>
       </c>
       <c r="C211" s="85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D211" s="29"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="B212" s="30" t="s">
         <v>283</v>
-      </c>
-      <c r="B212" s="30" t="s">
-        <v>284</v>
       </c>
       <c r="C212" s="30" t="s">
         <v>8</v>
@@ -4446,101 +4446,101 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B213" s="31">
         <v>1.66</v>
       </c>
       <c r="C213" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D213" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B214" s="31">
         <v>2</v>
       </c>
       <c r="C214" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D214" s="33"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B215" s="31">
         <v>3.3</v>
       </c>
       <c r="C215" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D215" s="33"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B216" s="34">
         <v>98.1</v>
       </c>
       <c r="C216" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D216" s="33"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B217" s="31">
         <v>1</v>
       </c>
       <c r="C217" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D217" s="33"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B218" s="35">
         <v>0.66</v>
       </c>
       <c r="C218" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D218" s="33"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B219" s="87">
         <v>0.3</v>
       </c>
       <c r="C219" s="87" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D219" s="32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="89" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B220" s="89">
         <v>0.3</v>
       </c>
       <c r="C220" s="90" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D220" s="88"/>
     </row>
@@ -4559,7 +4559,7 @@
       <formula1>"Very Light airplane, CS-23 airplane, CS-25 airplane"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{4759DC4D-4942-4CCB-9FB4-C98B79FBE93F}">
-      <formula1>"CSVLA, CS-23, CS-25"</formula1>
+      <formula1>"csvla, cs-23, cs-25"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{B1CA99B6-531C-4BD9-A2C9-62F759AF419E}">
       <formula1>"Single fin, Double fin, Multiple fin"</formula1>
@@ -4586,6 +4586,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ADEDA064E7272B44AAE37BAA6CD7FE3B" ma:contentTypeVersion="8" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="2d80b812441223625dff242ce84ff698">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5ed5f3a1-937f-4f8d-a024-7e291820fcff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a496629542ab54b55afabb88d9087217" ns2:_="">
     <xsd:import namespace="5ed5f3a1-937f-4f8d-a024-7e291820fcff"/>
@@ -4755,22 +4770,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D941D3B3-02DE-4D2A-81A9-FA0B5BB9B0E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5011C101-3E1F-41A7-9B66-51A81523BBF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{701D7F10-606B-4519-A327-4429D166EF78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4786,21 +4803,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5011C101-3E1F-41A7-9B66-51A81523BBF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D941D3B3-02DE-4D2A-81A9-FA0B5BB9B0E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>